<commit_message>
Updates: WIP ConfigurationManager and testConfigurationManager.
</commit_message>
<xml_diff>
--- a/misc/datafiles/implementation.xlsx
+++ b/misc/datafiles/implementation.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\YasserAlejandro\mtp\mtp-abm\misc\datafiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\YasserAlejandro\mp\mtp-abm\misc\datafiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,10 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
-  <si>
-    <t>client</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>BA</t>
   </si>
@@ -38,7 +35,19 @@
     <t>American</t>
   </si>
   <si>
-    <t>hours</t>
+    <t>icow</t>
+  </si>
+  <si>
+    <t>ihorse</t>
+  </si>
+  <si>
+    <t>iclient</t>
+  </si>
+  <si>
+    <t>ihours</t>
+  </si>
+  <si>
+    <t>itonto</t>
   </si>
 </sst>
 </file>
@@ -356,47 +365,83 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.28515625" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B1" t="s">
         <v>4</v>
       </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>3</v>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
       </c>
       <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2">
         <v>200</v>
       </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
         <v>1</v>
       </c>
       <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3">
         <v>100</v>
       </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>2</v>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1</v>
       </c>
       <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4">
         <v>500</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>